<commit_message>
grade update as of 10:07 AM Friday, January 3, 2025 (GMT+8) Time in 40 (Pob.)
</commit_message>
<xml_diff>
--- a/data/CE17_1L.xlsx
+++ b/data/CE17_1L.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\External Shiz\Programming\Grade Shower\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\External Shiz\Programming\Grade Shower\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C971B745-F1FC-42A0-B3E1-E78AA6A03432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5409A393-6663-4B5A-8A4D-F47F2001D684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1420,7 +1420,7 @@
         <v>100</v>
       </c>
       <c r="G8" s="1">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H8" s="4">
         <v>60</v>
@@ -1702,7 +1702,7 @@
         <v>70</v>
       </c>
       <c r="I18" s="4">
-        <v>53.33</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1722,13 +1722,13 @@
         <v>90</v>
       </c>
       <c r="F19" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G19" s="1">
         <v>95</v>
       </c>
       <c r="H19" s="4">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I19" s="4">
         <v>86.67</v>
@@ -1760,7 +1760,7 @@
         <v>70</v>
       </c>
       <c r="I20" s="4">
-        <v>53.33</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1789,7 +1789,7 @@
         <v>70</v>
       </c>
       <c r="I21" s="4">
-        <v>53.33</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1974,7 +1974,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D28" s="1">
         <v>40</v>
@@ -1992,7 +1992,7 @@
         <v>70</v>
       </c>
       <c r="I28" s="4">
-        <v>53.33</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2585,7 +2585,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3240,10 +3240,10 @@
         <v>68</v>
       </c>
       <c r="C23" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D23" s="1">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="E23" s="1">
         <v>60</v>

</xml_diff>